<commit_message>
Modification de la visibilité des description photo et contact
</commit_message>
<xml_diff>
--- a/Docs/Recommandation-SEO.xlsx
+++ b/Docs/Recommandation-SEO.xlsx
@@ -5,12 +5,15 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Recommandation" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Accessibilité" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">Recommandation!$A$1:$F$32</definedName>
+  </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
@@ -21,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="110">
   <si>
     <t xml:space="preserve">Catégorie</t>
   </si>
@@ -56,6 +59,9 @@
     <t xml:space="preserve">Utiliser une balise canonique</t>
   </si>
   <si>
+    <t xml:space="preserve">https://www.anthedesign.fr/referencement/balise-canonical-page-web/</t>
+  </si>
+  <si>
     <t xml:space="preserve">Nom de la page 2 n’est pas adéquat</t>
   </si>
   <si>
@@ -68,6 +74,9 @@
     <t xml:space="preserve">Renommé ‘’page2’’</t>
   </si>
   <si>
+    <t xml:space="preserve">https://developers.google.com/search/docs/beginner/seo-starter-guide?hl=fr</t>
+  </si>
+  <si>
     <t xml:space="preserve">SEO et Accessibilité – Faciliter la compréhension</t>
   </si>
   <si>
@@ -155,6 +164,9 @@
     <t xml:space="preserve">Rajouter les balises sémantique</t>
   </si>
   <si>
+    <t xml:space="preserve">https://blog.hubspot.fr/marketing/balises-semantiques</t>
+  </si>
+  <si>
     <t xml:space="preserve">SEO – Vitesse du site</t>
   </si>
   <si>
@@ -248,6 +260,9 @@
     <t xml:space="preserve">Supprimer cette balise avec ces mots clès</t>
   </si>
   <si>
+    <t xml:space="preserve">https://www.semjuice.com/definition/blacklist</t>
+  </si>
+  <si>
     <t xml:space="preserve">Dans le bas de page la liste des annuaires semble très bizarre</t>
   </si>
   <si>
@@ -290,6 +305,9 @@
     <t xml:space="preserve">Les ajouter</t>
   </si>
   <si>
+    <t xml:space="preserve">https://www.seoquantum.com/billet/balise-meta</t>
+  </si>
+  <si>
     <t xml:space="preserve">SEO – Contenu</t>
   </si>
   <si>
@@ -305,6 +323,12 @@
     <t xml:space="preserve">Créer des section comme ‘actualités’ par exemple</t>
   </si>
   <si>
+    <t xml:space="preserve">Légende :</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Recommandation réalisé</t>
+  </si>
+  <si>
     <t xml:space="preserve">Au niveau du bloc3, la couleur du texte est pratiquement la même que celle du fond, par conséquent le texte est peu lisible</t>
   </si>
   <si>
@@ -324,6 +348,12 @@
   </si>
   <si>
     <t xml:space="preserve">L’information  transmise par la couleur, doit être véhiculé par un autre moyen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Source</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://developer.mozilla.org/fr/docs/Web/Accessibility/Mobile_accessibility_checklist</t>
   </si>
 </sst>
 </file>
@@ -380,7 +410,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -401,20 +431,26 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FF81D41A"/>
+        <bgColor rgb="FF969696"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFDEDCE6"/>
         <bgColor rgb="FFDEE6EF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFF5CE"/>
+        <fgColor rgb="FFFAFAD2"/>
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFF5CE"/>
+        <bgColor rgb="FFFAFAD2"/>
       </patternFill>
     </fill>
     <fill>
@@ -488,7 +524,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="37">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -513,6 +549,10 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -521,15 +561,23 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -537,63 +585,43 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -601,20 +629,40 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="12" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="12" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="13" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -654,7 +702,7 @@
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF7030A0"/>
-      <rgbColor rgb="FFFFF5CE"/>
+      <rgbColor rgb="FFFAFAD2"/>
       <rgbColor rgb="FFDEE6EF"/>
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
@@ -678,7 +726,7 @@
       <rgbColor rgb="FFFFDBB6"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
-      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FF81D41A"/>
       <rgbColor rgb="FFFFCC00"/>
       <rgbColor rgb="FFFF9900"/>
       <rgbColor rgb="FFFF6600"/>
@@ -704,11 +752,11 @@
   </sheetPr>
   <dimension ref="A1:Z1003"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.4375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.50390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="38.35"/>
@@ -769,203 +817,230 @@
       <c r="C2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="7" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="39.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="F2" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="55.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="3"/>
       <c r="B3" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="D3" s="6" t="s">
         <v>14</v>
       </c>
+      <c r="E3" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E4" s="7"/>
+      <c r="E4" s="8"/>
     </row>
     <row r="5" customFormat="false" ht="32.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" s="9" t="s">
+      <c r="A5" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5" s="12"/>
+    </row>
+    <row r="6" customFormat="false" ht="76.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="9"/>
+      <c r="B6" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="E5" s="10" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="32.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="8"/>
-      <c r="B6" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="D6" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="E6" s="10" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="37.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="8"/>
-      <c r="B7" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="D7" s="9" t="s">
+    </row>
+    <row r="7" customFormat="false" ht="61.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="9"/>
+      <c r="B7" s="13" t="s">
         <v>26</v>
       </c>
+      <c r="C7" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>28</v>
+      </c>
       <c r="E7" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="F7" s="13"/>
+        <v>29</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="37.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="8"/>
-      <c r="B8" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="C8" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="D8" s="9" t="s">
+      <c r="A8" s="9"/>
+      <c r="B8" s="13" t="s">
         <v>30</v>
       </c>
+      <c r="C8" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>32</v>
+      </c>
       <c r="E8" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="F8" s="13"/>
-    </row>
-    <row r="9" customFormat="false" ht="38.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="8"/>
-      <c r="B9" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="C9" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="D9" s="9" t="s">
+      <c r="F8" s="12"/>
+    </row>
+    <row r="9" customFormat="false" ht="55.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="9"/>
+      <c r="B9" s="13" t="s">
         <v>34</v>
       </c>
+      <c r="C9" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>36</v>
+      </c>
       <c r="E9" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="F9" s="13"/>
+        <v>37</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="45.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="8"/>
-      <c r="B10" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="C10" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="D10" s="9" t="s">
+      <c r="A10" s="9"/>
+      <c r="B10" s="10" t="s">
         <v>38</v>
       </c>
+      <c r="C10" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>40</v>
+      </c>
       <c r="E10" s="12" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="8"/>
-      <c r="B11" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="C11" s="14" t="s">
         <v>41</v>
       </c>
+      <c r="F10" s="12"/>
+    </row>
+    <row r="11" customFormat="false" ht="52.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="9"/>
+      <c r="B11" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>43</v>
+      </c>
       <c r="D11" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="E11" s="15" t="s">
-        <v>43</v>
+        <v>44</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E12" s="7"/>
-    </row>
-    <row r="13" customFormat="false" ht="57.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E12" s="8"/>
+      <c r="F12" s="15"/>
+    </row>
+    <row r="13" customFormat="false" ht="74.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="16" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="B13" s="17" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="C13" s="17" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="D13" s="17" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="E13" s="18" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="32.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>51</v>
+      </c>
+      <c r="F13" s="18" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="60.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="16"/>
       <c r="B14" s="17" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="C14" s="17"/>
       <c r="D14" s="17" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="E14" s="18" t="s">
-        <v>51</v>
+        <v>54</v>
+      </c>
+      <c r="F14" s="18" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="67.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="16"/>
       <c r="B15" s="17" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C15" s="17" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="D15" s="17" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="E15" s="18" t="s">
-        <v>55</v>
-      </c>
+        <v>58</v>
+      </c>
+      <c r="F15" s="18"/>
     </row>
     <row r="16" customFormat="false" ht="34.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="16"/>
       <c r="B16" s="17" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="C16" s="17" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="D16" s="17" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="E16" s="18" t="s">
-        <v>59</v>
-      </c>
+        <v>62</v>
+      </c>
+      <c r="F16" s="18"/>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="19"/>
@@ -973,77 +1048,88 @@
       <c r="C17" s="20"/>
       <c r="D17" s="20"/>
       <c r="E17" s="21"/>
+      <c r="F17" s="15"/>
     </row>
     <row r="18" customFormat="false" ht="49.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="22" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="B18" s="23" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="C18" s="23" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="D18" s="23" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="E18" s="24" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="20" customFormat="false" ht="44" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>67</v>
+      </c>
+      <c r="F18" s="24"/>
+    </row>
+    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="F19" s="15"/>
+    </row>
+    <row r="20" customFormat="false" ht="56.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="25" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="B20" s="25" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="C20" s="25" t="s">
-        <v>67</v>
-      </c>
-      <c r="D20" s="25" t="s">
-        <v>68</v>
+        <v>70</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>71</v>
       </c>
       <c r="E20" s="25" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+        <v>72</v>
+      </c>
+      <c r="F20" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="F21" s="15"/>
+    </row>
     <row r="22" customFormat="false" ht="52.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="26" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="B22" s="27" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="C22" s="27" t="s">
-        <v>72</v>
-      </c>
-      <c r="D22" s="27" t="s">
-        <v>73</v>
+        <v>75</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>76</v>
       </c>
       <c r="E22" s="27" t="s">
-        <v>74</v>
-      </c>
-      <c r="F22" s="28"/>
+        <v>77</v>
+      </c>
+      <c r="F22" s="27" t="s">
+        <v>78</v>
+      </c>
       <c r="G22" s="28"/>
     </row>
     <row r="23" customFormat="false" ht="49.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="26"/>
       <c r="B23" s="27" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="C23" s="27" t="s">
-        <v>76</v>
-      </c>
-      <c r="D23" s="27" t="s">
-        <v>77</v>
+        <v>80</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>81</v>
       </c>
       <c r="E23" s="27" t="s">
-        <v>78</v>
-      </c>
-      <c r="F23" s="28"/>
+        <v>82</v>
+      </c>
+      <c r="F23" s="27"/>
       <c r="G23" s="28"/>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1052,63 +1138,81 @@
       <c r="C24" s="28"/>
       <c r="D24" s="28"/>
       <c r="E24" s="28"/>
+      <c r="F24" s="15"/>
     </row>
     <row r="25" customFormat="false" ht="48.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="29" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="B25" s="29" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="C25" s="29" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="D25" s="29" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="E25" s="29" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>87</v>
+      </c>
+      <c r="F25" s="29"/>
+    </row>
+    <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="F26" s="15"/>
+    </row>
+    <row r="27" customFormat="false" ht="70.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="30" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="B27" s="30" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="C27" s="30" t="s">
-        <v>86</v>
-      </c>
-      <c r="D27" s="30" t="s">
-        <v>87</v>
+        <v>90</v>
+      </c>
+      <c r="D27" s="14" t="s">
+        <v>91</v>
       </c>
       <c r="E27" s="30" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+        <v>92</v>
+      </c>
+      <c r="F27" s="31" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="F28" s="15"/>
+    </row>
     <row r="29" customFormat="false" ht="41.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="31" t="s">
-        <v>89</v>
-      </c>
-      <c r="B29" s="31" t="s">
-        <v>90</v>
-      </c>
-      <c r="C29" s="31" t="s">
-        <v>91</v>
-      </c>
-      <c r="D29" s="31" t="s">
-        <v>92</v>
-      </c>
-      <c r="E29" s="31" t="s">
-        <v>93</v>
-      </c>
+      <c r="A29" s="32" t="s">
+        <v>94</v>
+      </c>
+      <c r="B29" s="32" t="s">
+        <v>95</v>
+      </c>
+      <c r="C29" s="32" t="s">
+        <v>96</v>
+      </c>
+      <c r="D29" s="32" t="s">
+        <v>97</v>
+      </c>
+      <c r="E29" s="32" t="s">
+        <v>98</v>
+      </c>
+      <c r="F29" s="32"/>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="B32" s="33"/>
+      <c r="C32" s="34" t="s">
+        <v>100</v>
+      </c>
+    </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -2089,7 +2193,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="35" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2102,48 +2206,56 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G7" activeCellId="0" sqref="G7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="45.19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="36.03"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="32" t="s">
-        <v>94</v>
-      </c>
-      <c r="B1" s="32" t="s">
-        <v>95</v>
+      <c r="A1" s="35" t="s">
+        <v>101</v>
+      </c>
+      <c r="B1" s="35" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="33" t="s">
-        <v>96</v>
-      </c>
-      <c r="B2" s="32" t="s">
-        <v>95</v>
+      <c r="A2" s="36" t="s">
+        <v>103</v>
+      </c>
+      <c r="B2" s="35" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="33" t="s">
-        <v>99</v>
-      </c>
-      <c r="B4" s="33" t="s">
-        <v>100</v>
+      <c r="A4" s="36" t="s">
+        <v>106</v>
+      </c>
+      <c r="B4" s="36" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>109</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ajout title h2 dans page 2
</commit_message>
<xml_diff>
--- a/Docs/Recommandation-SEO.xlsx
+++ b/Docs/Recommandation-SEO.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="117">
   <si>
     <t xml:space="preserve">Catégorie</t>
   </si>
@@ -92,6 +92,9 @@
     <t xml:space="preserve">indiquer ‘’lang=fr’’</t>
   </si>
   <si>
+    <t xml:space="preserve">https://developer.mozilla.org/fr/docs/Web/HTML/Global_attributes/lang</t>
+  </si>
+  <si>
     <t xml:space="preserve">La balise description n’est pas remplie</t>
   </si>
   <si>
@@ -128,6 +131,9 @@
     <t xml:space="preserve">Rajouter un mot clé dans la balise ‘’h1’’</t>
   </si>
   <si>
+    <t xml:space="preserve">https://fiches-pratiques.chefdentreprise.com/Thematique/marketing-1052/FichePratique/Balise-h1-quel-est-son-interet--351214.htm</t>
+  </si>
+  <si>
     <t xml:space="preserve">Balise ‘’alt ‘’ mal remplie</t>
   </si>
   <si>
@@ -152,6 +158,9 @@
     <t xml:space="preserve">La supprimer</t>
   </si>
   <si>
+    <t xml:space="preserve">https://optimiz.me/definitions/la-balise-meta-keywords/</t>
+  </si>
+  <si>
     <t xml:space="preserve">Il manque les balise sémantique</t>
   </si>
   <si>
@@ -203,6 +212,9 @@
     <t xml:space="preserve">Augmenter la durée du cache sur 1 an</t>
   </si>
   <si>
+    <t xml:space="preserve">https://www.ionos.fr/digitalguide/hebergement/aspects-techniques/quest-ce-quun-cache/</t>
+  </si>
+  <si>
     <t xml:space="preserve">Le code HTML, CSS et quelque JS ne sont pas minifiés</t>
   </si>
   <si>
@@ -215,6 +227,9 @@
     <t xml:space="preserve">Minifier le code</t>
   </si>
   <si>
+    <t xml:space="preserve">https://talks.freelancerepublik.com/pourquoi-comment-minifier-code-source-web/</t>
+  </si>
+  <si>
     <t xml:space="preserve">SEO – Googlebot et JS</t>
   </si>
   <si>
@@ -230,6 +245,9 @@
     <t xml:space="preserve">Rajouter  l’attribut ‘defer’ aux balises JS</t>
   </si>
   <si>
+    <t xml:space="preserve">https://www.alsacreations.com/astuce/lire/1562-script-attribut-async-defer.html</t>
+  </si>
+  <si>
     <t xml:space="preserve">SEO – Responsive</t>
   </si>
   <si>
@@ -288,6 +306,9 @@
   </si>
   <si>
     <t xml:space="preserve">Placé les mots clés le plus souvent possible</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.brioude-internet.fr/7994/est-ce-que-je-peux-ecrire-du-texte-blanc-sur-fond-blanc/</t>
   </si>
   <si>
     <t xml:space="preserve">SEO – BACKLINK</t>
@@ -752,11 +773,11 @@
   </sheetPr>
   <dimension ref="A1:Z1003"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H18" activeCellId="0" sqref="H18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.50390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="38.35"/>
@@ -848,7 +869,7 @@
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="E4" s="8"/>
     </row>
-    <row r="5" customFormat="false" ht="32.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="73.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="9" t="s">
         <v>17</v>
       </c>
@@ -864,21 +885,23 @@
       <c r="E5" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="F5" s="12"/>
+      <c r="F5" s="12" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="76.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="9"/>
       <c r="B6" s="10" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F6" s="12" t="s">
         <v>16</v>
@@ -887,50 +910,52 @@
     <row r="7" customFormat="false" ht="61.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="9"/>
       <c r="B7" s="13" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F7" s="12" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="37.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="99.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="9"/>
       <c r="B8" s="13" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="F8" s="12"/>
+        <v>34</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="55.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="9"/>
       <c r="B9" s="13" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="F9" s="12" t="s">
         <v>16</v>
@@ -939,35 +964,37 @@
     <row r="10" customFormat="false" ht="45.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="9"/>
       <c r="B10" s="10" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="F10" s="12"/>
+        <v>43</v>
+      </c>
+      <c r="F10" s="12" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="52.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="9"/>
       <c r="B11" s="13" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="D11" s="14" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="F11" s="12" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -976,19 +1003,19 @@
     </row>
     <row r="13" customFormat="false" ht="74.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="16" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="B13" s="17" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="C13" s="17" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="D13" s="17" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="E13" s="18" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="F13" s="18" t="s">
         <v>16</v>
@@ -997,14 +1024,14 @@
     <row r="14" customFormat="false" ht="60.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="16"/>
       <c r="B14" s="17" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C14" s="17"/>
       <c r="D14" s="17" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="E14" s="18" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="F14" s="18" t="s">
         <v>16</v>
@@ -1013,34 +1040,38 @@
     <row r="15" customFormat="false" ht="67.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="16"/>
       <c r="B15" s="17" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="C15" s="17" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D15" s="17" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E15" s="18" t="s">
-        <v>58</v>
-      </c>
-      <c r="F15" s="18"/>
-    </row>
-    <row r="16" customFormat="false" ht="34.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>61</v>
+      </c>
+      <c r="F15" s="18" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="53.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="16"/>
       <c r="B16" s="17" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="C16" s="17" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="D16" s="17" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="E16" s="18" t="s">
-        <v>62</v>
-      </c>
-      <c r="F16" s="18"/>
+        <v>66</v>
+      </c>
+      <c r="F16" s="18" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="19"/>
@@ -1050,42 +1081,44 @@
       <c r="E17" s="21"/>
       <c r="F17" s="15"/>
     </row>
-    <row r="18" customFormat="false" ht="49.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="59.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="22" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="B18" s="23" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="C18" s="23" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="D18" s="23" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="E18" s="24" t="s">
-        <v>67</v>
-      </c>
-      <c r="F18" s="24"/>
+        <v>72</v>
+      </c>
+      <c r="F18" s="24" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="F19" s="15"/>
     </row>
     <row r="20" customFormat="false" ht="56.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="25" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="B20" s="25" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="C20" s="25" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="E20" s="25" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="F20" s="7" t="s">
         <v>16</v>
@@ -1096,38 +1129,38 @@
     </row>
     <row r="22" customFormat="false" ht="52.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="26" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="B22" s="27" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="C22" s="27" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="E22" s="27" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="F22" s="27" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="G22" s="28"/>
     </row>
     <row r="23" customFormat="false" ht="49.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="26"/>
       <c r="B23" s="27" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="C23" s="27" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="E23" s="27" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="F23" s="27"/>
       <c r="G23" s="28"/>
@@ -1140,45 +1173,47 @@
       <c r="E24" s="28"/>
       <c r="F24" s="15"/>
     </row>
-    <row r="25" customFormat="false" ht="48.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="73.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="29" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="B25" s="29" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="C25" s="29" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="D25" s="29" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="E25" s="29" t="s">
-        <v>87</v>
-      </c>
-      <c r="F25" s="29"/>
+        <v>93</v>
+      </c>
+      <c r="F25" s="29" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="F26" s="15"/>
     </row>
     <row r="27" customFormat="false" ht="70.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="30" t="s">
-        <v>88</v>
+        <v>95</v>
       </c>
       <c r="B27" s="30" t="s">
-        <v>89</v>
+        <v>96</v>
       </c>
       <c r="C27" s="30" t="s">
-        <v>90</v>
+        <v>97</v>
       </c>
       <c r="D27" s="14" t="s">
-        <v>91</v>
+        <v>98</v>
       </c>
       <c r="E27" s="30" t="s">
-        <v>92</v>
+        <v>99</v>
       </c>
       <c r="F27" s="31" t="s">
-        <v>93</v>
+        <v>100</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1186,19 +1221,19 @@
     </row>
     <row r="29" customFormat="false" ht="41.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="32" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="B29" s="32" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
       <c r="C29" s="32" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="D29" s="32" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
       <c r="E29" s="32" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="F29" s="32"/>
     </row>
@@ -1206,11 +1241,11 @@
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>99</v>
+        <v>106</v>
       </c>
       <c r="B32" s="33"/>
       <c r="C32" s="34" t="s">
-        <v>100</v>
+        <v>107</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -2212,7 +2247,7 @@
       <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.71484375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="45.19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="36.03"/>
@@ -2220,42 +2255,42 @@
   <sheetData>
     <row r="1" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="35" t="s">
-        <v>101</v>
+        <v>108</v>
       </c>
       <c r="B1" s="35" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="36" t="s">
-        <v>103</v>
+        <v>110</v>
       </c>
       <c r="B2" s="35" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>104</v>
+        <v>111</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>105</v>
+        <v>112</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="36" t="s">
-        <v>106</v>
+        <v>113</v>
       </c>
       <c r="B4" s="36" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>108</v>
+        <v>115</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>109</v>
+        <v>116</v>
       </c>
     </row>
   </sheetData>

</xml_diff>